<commit_message>
Ajustes a escaleta MA_10_06_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion06/ESCALETA_MA_10_06_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion06/ESCALETA_MA_10_06_CO.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado10\guion06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdrianaMa\Documents\GitHub\Matematicas\fuentes\contenidos\grado10\guion06\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22035" windowHeight="10785"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22032" windowHeight="10788"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -314,9 +314,6 @@
     <t>Recurso M9B-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para analizar y plantear la solución a situaciones  problema. </t>
-  </si>
-  <si>
     <t>Recurso M101A-03</t>
   </si>
   <si>
@@ -392,9 +389,6 @@
     <t xml:space="preserve">Actividad para determinar medidas de tendencia central en situaciones. </t>
   </si>
   <si>
-    <t xml:space="preserve">Actividad para determinar medidas de dispersión en situaciones. </t>
-  </si>
-  <si>
     <t>M5A</t>
   </si>
   <si>
@@ -509,9 +503,6 @@
     <t>Los tipos de muestreo</t>
   </si>
   <si>
-    <t>Interactivo para explicar los distintos tipos de muestreo en un estudio estadístico</t>
-  </si>
-  <si>
     <t>En la presentación inicial, presentar los distintos tipos de muestreo: aleatorio, sistemático, estratificado, por conglomerado, y otros. En cada menú explicar y pesentar ejemplo.</t>
   </si>
   <si>
@@ -521,21 +512,12 @@
     <t>Calcula las medidas de dispersión</t>
   </si>
   <si>
-    <t>Las medidas de posición</t>
-  </si>
-  <si>
-    <t>Interactivo para recordar cómo calcular las distintas medidas de posición: cuantiles: cuartiles, quintiles, deciles y percentiles</t>
-  </si>
-  <si>
     <t>Colombia grado 9</t>
   </si>
   <si>
     <t>Los cuartiles y el diagrama de caja y bigotes</t>
   </si>
   <si>
-    <t>Interactivo que permite a los alumnos conocer e interpretar el concepto de cuartil, diagrama de caja y bigotes y conocer sus aplicaciones</t>
-  </si>
-  <si>
     <t>Practica las medidas de posición</t>
   </si>
   <si>
@@ -557,9 +539,6 @@
     <t>Actividad para afianzar el significado de las medidas de dispersión estadística</t>
   </si>
   <si>
-    <t>La resolución de problemas mediante los diagramas de árbol</t>
-  </si>
-  <si>
     <t>Interactivo de gran utilidad para aprender a resolver problemas de combinatoria mediante diagramas de árbol</t>
   </si>
   <si>
@@ -581,9 +560,6 @@
     <t>Las magnitudes de la combinatoria</t>
   </si>
   <si>
-    <t>Interactivo que explica cómo se resuelven las variaciones, combinaciones y permutaciones, todas ellas con y sin repetición</t>
-  </si>
-  <si>
     <t>Resuelve problemas de combinatoria</t>
   </si>
   <si>
@@ -641,9 +617,6 @@
     <t>Banco de actividades sobre el tema La estadística y la combinatoria</t>
   </si>
   <si>
-    <t>Halla las combinaciones que pueden presentarse con o  sin repeticion</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
@@ -708,12 +681,39 @@
   </si>
   <si>
     <t>Recurso M8A-01</t>
+  </si>
+  <si>
+    <t>Interactivo que expone los distintos tipos de muestreo en un estudio estadístico</t>
+  </si>
+  <si>
+    <t>Interactivo que muestra cómo calcular los distintos cuantiles: cuartiles, quintiles, deciles y percentiles</t>
+  </si>
+  <si>
+    <t>Interactivo para conocer e interpretar el concepto de cuartil, diagrama de caja y bigotes y sus aplicaciones</t>
+  </si>
+  <si>
+    <t>Actividad para determinar medidas de dispersión en situaciones</t>
+  </si>
+  <si>
+    <t>Actividad para analizar y plantear la solución estadística a situaciones problema</t>
+  </si>
+  <si>
+    <t>Interactivo que aplica las fórmulas para resolver las variaciones, combinaciones y permutaciones, con y sin repetición</t>
+  </si>
+  <si>
+    <t>Resuelve problemas mediante los diagramas de árbol</t>
+  </si>
+  <si>
+    <t>Practica las permutaciones sin repetición</t>
+  </si>
+  <si>
+    <t>Resuelve combinaciones con y sin repeticion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -955,7 +955,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1125,12 +1125,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1140,53 +1188,8 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1281,23 +1284,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1333,23 +1319,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1530,145 +1499,145 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19:E20"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="47.59765625" defaultRowHeight="15.85" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="47.5546875" defaultRowHeight="15.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="4" max="4" width="29.73046875" customWidth="1"/>
-    <col min="5" max="5" width="29.265625" customWidth="1"/>
-    <col min="6" max="6" width="25.1328125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="47.86328125" customWidth="1"/>
-    <col min="8" max="8" width="21.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="25.73046875" customWidth="1"/>
-    <col min="12" max="12" width="29.265625" customWidth="1"/>
-    <col min="13" max="13" width="20.265625" customWidth="1"/>
-    <col min="14" max="14" width="19.265625" customWidth="1"/>
-    <col min="15" max="15" width="47.59765625" style="1"/>
+    <col min="4" max="4" width="29.77734375" customWidth="1"/>
+    <col min="5" max="5" width="29.21875" customWidth="1"/>
+    <col min="6" max="6" width="25.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="47.88671875" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="25.77734375" customWidth="1"/>
+    <col min="12" max="12" width="29.21875" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="19.21875" customWidth="1"/>
+    <col min="15" max="15" width="47.5546875" style="1"/>
     <col min="16" max="16" width="28" style="1" customWidth="1"/>
-    <col min="17" max="17" width="23.265625" style="48" customWidth="1"/>
-    <col min="18" max="18" width="22.59765625" style="44" customWidth="1"/>
-    <col min="19" max="19" width="20.1328125" style="44" customWidth="1"/>
-    <col min="20" max="20" width="23.73046875" style="44" customWidth="1"/>
-    <col min="21" max="21" width="20.73046875" style="44" customWidth="1"/>
-    <col min="22" max="22" width="18.73046875" style="44" customWidth="1"/>
-    <col min="23" max="23" width="32.86328125" style="44" customWidth="1"/>
+    <col min="17" max="17" width="23.21875" style="48" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" style="44" customWidth="1"/>
+    <col min="19" max="19" width="20.109375" style="44" customWidth="1"/>
+    <col min="20" max="20" width="23.77734375" style="44" customWidth="1"/>
+    <col min="21" max="21" width="20.77734375" style="44" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" style="44" customWidth="1"/>
+    <col min="23" max="23" width="32.88671875" style="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="5" customFormat="1" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:23" s="5" customFormat="1" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="78" t="s">
+      <c r="C1" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="73" t="s">
+      <c r="K1" s="70" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="71" t="s">
+      <c r="L1" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="76" t="s">
+      <c r="M1" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="76"/>
-      <c r="O1" s="59" t="s">
+      <c r="N1" s="73"/>
+      <c r="O1" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="59" t="s">
+      <c r="P1" s="62" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="61" t="s">
+      <c r="Q1" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="61" t="s">
+      <c r="S1" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="62" t="s">
+      <c r="T1" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="61" t="s">
+      <c r="U1" s="77" t="s">
         <v>69</v>
       </c>
       <c r="V1" s="57"/>
       <c r="W1" s="57"/>
     </row>
-    <row r="2" spans="1:23" s="5" customFormat="1" ht="15.85" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="70"/>
-      <c r="B2" s="68"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="77"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="72"/>
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="15.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="67"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="69"/>
       <c r="M2" s="6" t="s">
         <v>70</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="60"/>
-      <c r="P2" s="60"/>
-      <c r="Q2" s="61"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="61"/>
-      <c r="T2" s="62"/>
-      <c r="U2" s="61"/>
+      <c r="O2" s="63"/>
+      <c r="P2" s="63"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="77"/>
       <c r="V2" s="57"/>
       <c r="W2" s="57"/>
     </row>
-    <row r="3" spans="1:23" s="5" customFormat="1" ht="15.85" customHeight="1" thickTop="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:23" s="5" customFormat="1" ht="15.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="30"/>
       <c r="G3" s="31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="H3" s="28">
         <v>1</v>
@@ -1677,7 +1646,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K3" s="23" t="s">
         <v>19</v>
@@ -1688,46 +1657,46 @@
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
       <c r="O3" s="36" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P3" s="36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q3" s="50">
         <v>10</v>
       </c>
       <c r="R3" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S3" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T3" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="U3" s="50" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="V3" s="57"/>
       <c r="W3" s="57"/>
     </row>
-    <row r="4" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="9"/>
       <c r="G4" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H4" s="9">
         <v>2</v>
@@ -1736,7 +1705,7 @@
         <v>19</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>19</v>
@@ -1747,52 +1716,52 @@
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
       <c r="O4" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P4" s="36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q4" s="45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="R4" s="46" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="S4" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T4" s="47" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="U4" s="45" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="V4" s="58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="W4" s="58" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E5" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H5" s="13">
         <v>3</v>
@@ -1801,7 +1770,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="K5" s="23" t="s">
         <v>20</v>
@@ -1811,10 +1780,10 @@
       </c>
       <c r="M5" s="15"/>
       <c r="N5" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O5" s="16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P5" s="12" t="s">
         <v>19</v>
@@ -1835,25 +1804,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B6" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E6" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F6" s="13"/>
       <c r="G6" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H6" s="26">
         <v>4</v>
@@ -1862,7 +1831,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K6" s="23" t="s">
         <v>20</v>
@@ -1872,10 +1841,10 @@
       </c>
       <c r="M6" s="15"/>
       <c r="N6" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="P6" s="12" t="s">
         <v>19</v>
@@ -1896,25 +1865,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E7" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H7" s="9">
         <v>5</v>
@@ -1923,7 +1892,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K7" s="23" t="s">
         <v>19</v>
@@ -1934,54 +1903,54 @@
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
       <c r="O7" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>20</v>
       </c>
       <c r="Q7" s="45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="R7" s="46" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="S7" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T7" s="47" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="U7" s="45" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="V7" s="58" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="W7" s="58" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E8" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>92</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H8" s="13">
         <v>6</v>
@@ -1990,7 +1959,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K8" s="23" t="s">
         <v>20</v>
@@ -2000,10 +1969,10 @@
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O8" s="16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P8" s="12" t="s">
         <v>19</v>
@@ -2018,33 +1987,33 @@
         <v>89</v>
       </c>
       <c r="T8" s="54" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="U8" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E9" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H9" s="26">
         <v>7</v>
@@ -2053,7 +2022,7 @@
         <v>19</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>20</v>
@@ -2066,7 +2035,7 @@
       </c>
       <c r="N9" s="15"/>
       <c r="O9" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="P9" s="12" t="s">
         <v>19</v>
@@ -2081,31 +2050,31 @@
         <v>86</v>
       </c>
       <c r="T9" s="55" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="U9" s="50" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="17" t="s">
         <v>104</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>105</v>
       </c>
       <c r="F10" s="13"/>
       <c r="G10" s="14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H10" s="9">
         <v>8</v>
@@ -2114,7 +2083,7 @@
         <v>20</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>20</v>
@@ -2124,10 +2093,10 @@
       </c>
       <c r="M10" s="15"/>
       <c r="N10" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O10" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P10" s="12" t="s">
         <v>19</v>
@@ -2142,33 +2111,33 @@
         <v>89</v>
       </c>
       <c r="T10" s="54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="U10" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="13" t="s">
         <v>92</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H11" s="13">
         <v>9</v>
@@ -2177,7 +2146,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K11" s="23" t="s">
         <v>20</v>
@@ -2187,10 +2156,10 @@
       </c>
       <c r="M11" s="15"/>
       <c r="N11" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O11" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="P11" s="12" t="s">
         <v>19</v>
@@ -2211,25 +2180,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E12" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="F12" s="13"/>
       <c r="G12" s="14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H12" s="26">
         <v>10</v>
@@ -2238,7 +2207,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K12" s="23" t="s">
         <v>20</v>
@@ -2248,10 +2217,10 @@
       </c>
       <c r="M12" s="15"/>
       <c r="N12" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O12" s="16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P12" s="12" t="s">
         <v>19</v>
@@ -2272,25 +2241,25 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E13" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="14" t="s">
-        <v>165</v>
+        <v>207</v>
       </c>
       <c r="H13" s="9">
         <v>11</v>
@@ -2299,7 +2268,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>166</v>
+        <v>220</v>
       </c>
       <c r="K13" s="23" t="s">
         <v>19</v>
@@ -2310,52 +2279,52 @@
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
       <c r="O13" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P13" s="12" t="s">
         <v>20</v>
       </c>
       <c r="Q13" s="45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="R13" s="46" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="S13" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T13" s="47" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="U13" s="45" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="V13" s="58" t="s">
         <v>70</v>
       </c>
       <c r="W13" s="58" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E14" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="39" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H14" s="13">
         <v>12</v>
@@ -2363,8 +2332,8 @@
       <c r="I14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="38" t="s">
-        <v>169</v>
+      <c r="J14" s="80" t="s">
+        <v>221</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>19</v>
@@ -2375,52 +2344,52 @@
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
       <c r="O14" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="Q14" s="45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="R14" s="46" t="s">
+        <v>200</v>
+      </c>
+      <c r="S14" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="T14" s="47" t="s">
+        <v>163</v>
+      </c>
+      <c r="U14" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="V14" s="58" t="s">
+        <v>122</v>
+      </c>
+      <c r="W14" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="S14" s="45" t="s">
-        <v>104</v>
-      </c>
-      <c r="T14" s="47" t="s">
-        <v>168</v>
-      </c>
-      <c r="U14" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="V14" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="W14" s="58" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="15" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E15" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="39" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="H15" s="26">
         <v>13</v>
@@ -2429,7 +2398,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="K15" s="23" t="s">
         <v>20</v>
@@ -2442,7 +2411,7 @@
         <v>37</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="P15" s="12" t="s">
         <v>19</v>
@@ -2457,31 +2426,31 @@
         <v>89</v>
       </c>
       <c r="T15" s="54" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="U15" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E16" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="14" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H16" s="9">
         <v>14</v>
@@ -2490,7 +2459,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>122</v>
+        <v>222</v>
       </c>
       <c r="K16" s="23" t="s">
         <v>20</v>
@@ -2503,7 +2472,7 @@
         <v>40</v>
       </c>
       <c r="O16" s="16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="P16" s="12" t="s">
         <v>19</v>
@@ -2518,31 +2487,31 @@
         <v>89</v>
       </c>
       <c r="T16" s="54" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="U16" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E17" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="14" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="H17" s="13">
         <v>15</v>
@@ -2551,7 +2520,7 @@
         <v>19</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>19</v>
@@ -2562,52 +2531,52 @@
       <c r="M17" s="37"/>
       <c r="N17" s="37"/>
       <c r="O17" s="16" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="P17" s="12" t="s">
         <v>19</v>
       </c>
       <c r="Q17" s="45" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="R17" s="46" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="S17" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T17" s="47" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="U17" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="V17" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="W17" s="58" t="s">
         <v>211</v>
       </c>
-      <c r="V17" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="W17" s="58" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="18" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="E18" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="14" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="H18" s="26">
         <v>16</v>
@@ -2616,7 +2585,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>19</v>
@@ -2627,7 +2596,7 @@
       <c r="M18" s="37"/>
       <c r="N18" s="37"/>
       <c r="O18" s="16" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="P18" s="12" t="s">
         <v>20</v>
@@ -2636,37 +2605,37 @@
         <v>10</v>
       </c>
       <c r="R18" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S18" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="T18" s="51" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="U18" s="50" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>92</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H19" s="9">
         <v>17</v>
@@ -2675,7 +2644,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="14" t="s">
-        <v>96</v>
+        <v>223</v>
       </c>
       <c r="K19" s="23" t="s">
         <v>20</v>
@@ -2685,10 +2654,10 @@
       </c>
       <c r="M19" s="15"/>
       <c r="N19" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O19" s="16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P19" s="12" t="s">
         <v>19</v>
@@ -2703,31 +2672,31 @@
         <v>89</v>
       </c>
       <c r="T19" s="54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U19" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E20" s="17" t="s">
         <v>92</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="14" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H20" s="13">
         <v>18</v>
@@ -2736,7 +2705,7 @@
         <v>19</v>
       </c>
       <c r="J20" s="56" t="s">
-        <v>185</v>
+        <v>224</v>
       </c>
       <c r="K20" s="23" t="s">
         <v>19</v>
@@ -2754,57 +2723,57 @@
         <v>10</v>
       </c>
       <c r="R20" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S20" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T20" s="51" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="U20" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F21" s="13"/>
       <c r="G21" s="14" t="s">
-        <v>177</v>
+        <v>225</v>
       </c>
       <c r="H21" s="26">
         <v>19</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>19</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="M21" s="35"/>
       <c r="N21" s="35"/>
       <c r="O21" s="16" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="P21" s="12" t="s">
         <v>19</v>
@@ -2813,37 +2782,37 @@
         <v>10</v>
       </c>
       <c r="R21" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S21" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T21" s="51" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="U21" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="13"/>
       <c r="G22" s="14" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="H22" s="9">
         <v>20</v>
@@ -2852,7 +2821,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="K22" s="23" t="s">
         <v>19</v>
@@ -2863,7 +2832,7 @@
       <c r="M22" s="35"/>
       <c r="N22" s="35"/>
       <c r="O22" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P22" s="12" t="s">
         <v>19</v>
@@ -2872,37 +2841,37 @@
         <v>10</v>
       </c>
       <c r="R22" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S22" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T22" s="51" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="U22" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="14" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="H23" s="13">
         <v>21</v>
@@ -2911,7 +2880,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="14" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="K23" s="23" t="s">
         <v>19</v>
@@ -2922,7 +2891,7 @@
       <c r="M23" s="35"/>
       <c r="N23" s="35"/>
       <c r="O23" s="16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="P23" s="12" t="s">
         <v>19</v>
@@ -2931,37 +2900,37 @@
         <v>10</v>
       </c>
       <c r="R23" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S23" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T23" s="51" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="U23" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F24" s="13"/>
       <c r="G24" s="14" t="s">
-        <v>194</v>
+        <v>226</v>
       </c>
       <c r="H24" s="26">
         <v>22</v>
@@ -2970,7 +2939,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="14" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="K24" s="23" t="s">
         <v>19</v>
@@ -2981,7 +2950,7 @@
       <c r="M24" s="35"/>
       <c r="N24" s="35"/>
       <c r="O24" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="P24" s="12" t="s">
         <v>19</v>
@@ -2990,37 +2959,37 @@
         <v>10</v>
       </c>
       <c r="R24" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S24" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T24" s="51" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="U24" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F25" s="13"/>
       <c r="G25" s="14" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="H25" s="9">
         <v>23</v>
@@ -3029,7 +2998,7 @@
         <v>19</v>
       </c>
       <c r="J25" s="14" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="K25" s="23" t="s">
         <v>19</v>
@@ -3047,37 +3016,37 @@
         <v>10</v>
       </c>
       <c r="R25" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S25" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T25" s="51" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="U25" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="14" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="H26" s="13">
         <v>24</v>
@@ -3086,7 +3055,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="14" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="K26" s="23" t="s">
         <v>20</v>
@@ -3096,7 +3065,7 @@
       </c>
       <c r="M26" s="15"/>
       <c r="N26" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O26" s="16"/>
       <c r="P26" s="12" t="s">
@@ -3112,31 +3081,31 @@
         <v>89</v>
       </c>
       <c r="T26" s="54" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="U26" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="39" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="H27" s="26">
         <v>25</v>
@@ -3145,7 +3114,7 @@
         <v>19</v>
       </c>
       <c r="J27" s="40" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="K27" s="23" t="s">
         <v>19</v>
@@ -3163,37 +3132,37 @@
         <v>10</v>
       </c>
       <c r="R27" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S27" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T27" s="51" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="U27" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="39" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="H28" s="9">
         <v>26</v>
@@ -3202,7 +3171,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="40" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="K28" s="23" t="s">
         <v>19</v>
@@ -3220,37 +3189,37 @@
         <v>10</v>
       </c>
       <c r="R28" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S28" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T28" s="51" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="U28" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>92</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="14" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="H29" s="13">
         <v>27</v>
@@ -3259,7 +3228,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="14" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>20</v>
@@ -3269,10 +3238,10 @@
       </c>
       <c r="M29" s="15"/>
       <c r="N29" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O29" s="16" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P29" s="12" t="s">
         <v>19</v>
@@ -3287,29 +3256,29 @@
         <v>86</v>
       </c>
       <c r="T29" s="54" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="U29" s="52" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="13"/>
       <c r="G30" s="22" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="H30" s="26">
         <v>28</v>
@@ -3318,7 +3287,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>19</v>
@@ -3331,7 +3300,7 @@
         <v>83</v>
       </c>
       <c r="O30" s="21" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P30" s="12" t="s">
         <v>19</v>
@@ -3340,30 +3309,30 @@
         <v>10</v>
       </c>
       <c r="R30" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S30" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T30" s="51" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="U30" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>10</v>
@@ -3379,7 +3348,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="14" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>20</v>
@@ -3399,25 +3368,25 @@
       <c r="T31" s="47"/>
       <c r="U31" s="45"/>
     </row>
-    <row r="32" spans="1:23" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:23" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D32" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="17" t="s">
         <v>99</v>
-      </c>
-      <c r="E32" s="17" t="s">
-        <v>100</v>
       </c>
       <c r="F32" s="13"/>
       <c r="G32" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H32" s="13">
         <v>30</v>
@@ -3426,7 +3395,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="14" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="K32" s="23" t="s">
         <v>20</v>
@@ -3436,10 +3405,10 @@
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O32" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P32" s="12" t="s">
         <v>19</v>
@@ -3454,31 +3423,31 @@
         <v>89</v>
       </c>
       <c r="T32" s="54" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="U32" s="52" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="15.85" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:21" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H33" s="26">
         <v>31</v>
@@ -3487,7 +3456,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="14" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="K33" s="23" t="s">
         <v>19</v>
@@ -3500,7 +3469,7 @@
         <v>52</v>
       </c>
       <c r="O33" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P33" s="12" t="s">
         <v>20</v>
@@ -3509,22 +3478,22 @@
         <v>10</v>
       </c>
       <c r="R33" s="49" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="S33" s="50" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="T33" s="51" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="U33" s="50" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H34" s="41"/>
     </row>
-    <row r="35" spans="1:21" ht="15.85" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:21" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H35" s="41"/>
     </row>
   </sheetData>
@@ -3532,6 +3501,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3546,12 +3521,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3602,27 +3571,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="2" customWidth="1"/>
     <col min="4" max="4" width="34" style="2" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="34.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.77734375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" style="2" customWidth="1"/>
     <col min="12" max="12" width="17" style="2" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="2"/>
-    <col min="14" max="14" width="24.265625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="2"/>
+    <col min="13" max="13" width="11.44140625" style="2"/>
+    <col min="14" max="14" width="24.21875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="69.88671875" style="2" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -3639,7 +3608,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -3663,7 +3632,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -3682,7 +3651,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -3701,7 +3670,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3717,7 +3686,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -3734,7 +3703,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -3751,7 +3720,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -3766,7 +3735,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -3781,7 +3750,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -3796,7 +3765,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -3811,7 +3780,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -3826,7 +3795,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -3841,7 +3810,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -3856,7 +3825,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -3871,7 +3840,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -3886,7 +3855,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="2" t="s">
@@ -3900,7 +3869,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
@@ -3914,7 +3883,7 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
@@ -3928,7 +3897,7 @@
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="2" t="s">
@@ -3942,7 +3911,7 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3957,7 +3926,7 @@
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -3972,7 +3941,7 @@
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -3987,7 +3956,7 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -4002,7 +3971,7 @@
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -4017,7 +3986,7 @@
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -4032,7 +4001,7 @@
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -4047,7 +4016,7 @@
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -4062,7 +4031,7 @@
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -4077,7 +4046,7 @@
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -4092,7 +4061,7 @@
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -4107,7 +4076,7 @@
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -4122,7 +4091,7 @@
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -4137,7 +4106,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -4152,7 +4121,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -4167,7 +4136,7 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -4182,7 +4151,7 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -4197,7 +4166,7 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -4212,7 +4181,7 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -4227,7 +4196,7 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -4242,7 +4211,7 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -4257,7 +4226,7 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -4272,7 +4241,7 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -4287,7 +4256,7 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -4302,7 +4271,7 @@
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -4317,7 +4286,7 @@
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -4332,7 +4301,7 @@
       <c r="K46" s="3"/>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -4347,7 +4316,7 @@
       <c r="K47" s="3"/>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -4362,7 +4331,7 @@
       <c r="K48" s="3"/>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -4374,7 +4343,7 @@
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -4386,7 +4355,7 @@
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -4399,7 +4368,7 @@
       <c r="K51" s="3"/>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -4412,7 +4381,7 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -4425,7 +4394,7 @@
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -4438,7 +4407,7 @@
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -4451,7 +4420,7 @@
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -4464,7 +4433,7 @@
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -4477,7 +4446,7 @@
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -4490,7 +4459,7 @@
       <c r="K58" s="3"/>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -4503,7 +4472,7 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -4516,7 +4485,7 @@
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -4529,7 +4498,7 @@
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -4542,7 +4511,7 @@
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -4555,7 +4524,7 @@
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -4568,7 +4537,7 @@
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -4581,7 +4550,7 @@
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -4594,7 +4563,7 @@
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -4607,7 +4576,7 @@
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -4620,7 +4589,7 @@
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -4633,7 +4602,7 @@
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -4646,7 +4615,7 @@
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4660,7 +4629,7 @@
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4674,7 +4643,7 @@
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4688,7 +4657,7 @@
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -4702,7 +4671,7 @@
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -4716,7 +4685,7 @@
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -4730,7 +4699,7 @@
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -4744,7 +4713,7 @@
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -4758,7 +4727,7 @@
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -4772,7 +4741,7 @@
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -4786,7 +4755,7 @@
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -4800,7 +4769,7 @@
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -4814,7 +4783,7 @@
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -4828,7 +4797,7 @@
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -4842,7 +4811,7 @@
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -4856,7 +4825,7 @@
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -4870,7 +4839,7 @@
       <c r="K86" s="3"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -4884,7 +4853,7 @@
       <c r="K87" s="3"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -4898,7 +4867,7 @@
       <c r="K88" s="3"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -4912,7 +4881,7 @@
       <c r="K89" s="3"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -4926,7 +4895,7 @@
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -4940,7 +4909,7 @@
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -4954,7 +4923,7 @@
       <c r="K92" s="3"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -4968,7 +4937,7 @@
       <c r="K93" s="3"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -4982,7 +4951,7 @@
       <c r="K94" s="3"/>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -4996,7 +4965,7 @@
       <c r="K95" s="3"/>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5010,7 +4979,7 @@
       <c r="K96" s="3"/>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5024,7 +4993,7 @@
       <c r="K97" s="3"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5038,7 +5007,7 @@
       <c r="K98" s="3"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5052,7 +5021,7 @@
       <c r="K99" s="3"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -5066,7 +5035,7 @@
       <c r="K100" s="3"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -5080,7 +5049,7 @@
       <c r="K101" s="3"/>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -5094,7 +5063,7 @@
       <c r="K102" s="3"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -5108,7 +5077,7 @@
       <c r="K103" s="3"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -5122,7 +5091,7 @@
       <c r="K104" s="3"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -5136,7 +5105,7 @@
       <c r="K105" s="3"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -5150,7 +5119,7 @@
       <c r="K106" s="3"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -5164,7 +5133,7 @@
       <c r="K107" s="3"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -5178,7 +5147,7 @@
       <c r="K108" s="3"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -5192,7 +5161,7 @@
       <c r="K109" s="3"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
@@ -5206,7 +5175,7 @@
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
@@ -5220,7 +5189,7 @@
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
@@ -5234,7 +5203,7 @@
       <c r="K112" s="3"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
@@ -5248,7 +5217,7 @@
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
@@ -5262,7 +5231,7 @@
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
@@ -5276,7 +5245,7 @@
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
@@ -5290,7 +5259,7 @@
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
@@ -5304,7 +5273,7 @@
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
@@ -5318,7 +5287,7 @@
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
@@ -5332,7 +5301,7 @@
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
@@ -5346,7 +5315,7 @@
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -5360,7 +5329,7 @@
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -5374,7 +5343,7 @@
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -5388,7 +5357,7 @@
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -5402,7 +5371,7 @@
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -5416,7 +5385,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -5430,7 +5399,7 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -5444,7 +5413,7 @@
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -5458,7 +5427,7 @@
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="3"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
@@ -5472,7 +5441,7 @@
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="3"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
@@ -5486,7 +5455,7 @@
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
@@ -5500,7 +5469,7 @@
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="3"/>
       <c r="B132" s="3"/>
       <c r="C132" s="3"/>
@@ -5514,7 +5483,7 @@
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="3"/>
       <c r="B133" s="3"/>
       <c r="C133" s="3"/>

</xml_diff>